<commit_message>
changed col names in Monthes
</commit_message>
<xml_diff>
--- a/util-res-task/monthly_target_dates_accum_df_0.xlsx
+++ b/util-res-task/monthly_target_dates_accum_df_0.xlsx
@@ -441,22 +441,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">M1 - </t>
+          <t>M1 - Ramhadam</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">M2 - </t>
+          <t>M2 - Shawwal</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">M3 - </t>
+          <t>M3 - Dhu al-Qi’dah</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">M4 - </t>
+          <t>M4 - Dhu al-Hijjah</t>
         </is>
       </c>
     </row>

</xml_diff>